<commit_message>
council spreadsheet change only
</commit_message>
<xml_diff>
--- a/results/council-workbook.xlsx
+++ b/results/council-workbook.xlsx
@@ -319,8 +319,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="57">
+  <cellStyleXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -383,7 +385,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="57">
+  <cellStyles count="59">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -412,6 +414,7 @@
     <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -440,6 +443,7 @@
     <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="57" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -772,7 +776,7 @@
   <dimension ref="A1:G40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0"/>
@@ -814,10 +818,10 @@
         <v>15</v>
       </c>
       <c r="E2">
-        <v>0.22</v>
+        <v>0.2</v>
       </c>
       <c r="F2">
-        <v>51756</v>
+        <v>1234567</v>
       </c>
       <c r="G2" t="b">
         <v>0</v>
@@ -837,10 +841,10 @@
         <v>20</v>
       </c>
       <c r="E3">
-        <v>0.41</v>
+        <v>0.3</v>
       </c>
       <c r="F3">
-        <v>11111</v>
+        <v>123456</v>
       </c>
       <c r="G3" t="b">
         <v>0</v>
@@ -860,10 +864,10 @@
         <v>14</v>
       </c>
       <c r="E4">
-        <v>0.22</v>
+        <v>0.4</v>
       </c>
       <c r="F4">
-        <v>51756</v>
+        <v>12345</v>
       </c>
       <c r="G4" t="b">
         <v>0</v>
@@ -883,10 +887,10 @@
         <v>13</v>
       </c>
       <c r="E5">
-        <v>0.41</v>
+        <v>0.1</v>
       </c>
       <c r="F5">
-        <v>11111</v>
+        <v>1234</v>
       </c>
       <c r="G5" t="b">
         <v>0</v>
@@ -906,10 +910,10 @@
         <v>9</v>
       </c>
       <c r="E6">
-        <v>0.22</v>
+        <v>0</v>
       </c>
       <c r="F6">
-        <v>51756</v>
+        <v>123</v>
       </c>
       <c r="G6" t="b">
         <v>0</v>
@@ -929,10 +933,10 @@
         <v>9</v>
       </c>
       <c r="E7">
-        <v>0.41</v>
+        <v>0.4</v>
       </c>
       <c r="F7">
-        <v>11111</v>
+        <v>12345</v>
       </c>
       <c r="G7" t="b">
         <v>0</v>
@@ -952,10 +956,10 @@
         <v>13</v>
       </c>
       <c r="E8">
-        <v>0.22</v>
+        <v>0.6</v>
       </c>
       <c r="F8">
-        <v>51756</v>
+        <v>123</v>
       </c>
       <c r="G8" t="b">
         <v>0</v>
@@ -975,10 +979,10 @@
         <v>9</v>
       </c>
       <c r="E9">
-        <v>0.41</v>
+        <v>0.7</v>
       </c>
       <c r="F9">
-        <v>11111</v>
+        <v>123678</v>
       </c>
       <c r="G9" t="b">
         <v>0</v>
@@ -998,10 +1002,10 @@
         <v>13</v>
       </c>
       <c r="E10">
-        <v>0.22</v>
+        <v>0.3</v>
       </c>
       <c r="F10">
-        <v>51756</v>
+        <v>123</v>
       </c>
       <c r="G10" t="b">
         <v>0</v>
@@ -1021,10 +1025,10 @@
         <v>9</v>
       </c>
       <c r="E11">
-        <v>0.41</v>
+        <v>0.66</v>
       </c>
       <c r="F11">
-        <v>11111</v>
+        <v>56789</v>
       </c>
       <c r="G11" t="b">
         <v>0</v>
@@ -1044,10 +1048,10 @@
         <v>14</v>
       </c>
       <c r="E12">
-        <v>0.22</v>
+        <v>0.34</v>
       </c>
       <c r="F12">
-        <v>51756</v>
+        <v>123</v>
       </c>
       <c r="G12" t="b">
         <v>0</v>
@@ -1067,10 +1071,10 @@
         <v>13</v>
       </c>
       <c r="E13">
-        <v>0.41</v>
+        <v>0.4</v>
       </c>
       <c r="F13">
-        <v>11111</v>
+        <v>469</v>
       </c>
       <c r="G13" t="b">
         <v>0</v>
@@ -1090,10 +1094,10 @@
         <v>9</v>
       </c>
       <c r="E14">
-        <v>0.22</v>
+        <v>0.6</v>
       </c>
       <c r="F14">
-        <v>51756</v>
+        <v>136</v>
       </c>
       <c r="G14" t="b">
         <v>0</v>
@@ -1116,7 +1120,7 @@
         <v>0.41</v>
       </c>
       <c r="F15">
-        <v>11111</v>
+        <v>56789</v>
       </c>
       <c r="G15" t="b">
         <v>0</v>
@@ -1136,13 +1140,13 @@
         <v>14</v>
       </c>
       <c r="E16">
-        <v>0.22</v>
+        <v>0.59</v>
       </c>
       <c r="F16">
-        <v>51756</v>
+        <v>987</v>
       </c>
       <c r="G16" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:7">
@@ -1159,10 +1163,10 @@
         <v>9</v>
       </c>
       <c r="E17">
-        <v>0.41</v>
+        <v>0.4</v>
       </c>
       <c r="F17">
-        <v>11111</v>
+        <v>345</v>
       </c>
       <c r="G17" s="2" t="b">
         <v>0</v>
@@ -1182,10 +1186,10 @@
         <v>13</v>
       </c>
       <c r="E18">
-        <v>0.22</v>
+        <v>0.2</v>
       </c>
       <c r="F18">
-        <v>51756</v>
+        <v>567</v>
       </c>
       <c r="G18" s="2" t="b">
         <v>0</v>
@@ -1205,10 +1209,10 @@
         <v>15</v>
       </c>
       <c r="E19">
-        <v>0.41</v>
+        <v>0.4</v>
       </c>
       <c r="F19">
-        <v>11111</v>
+        <v>765</v>
       </c>
       <c r="G19" s="2" t="b">
         <v>0</v>
@@ -1228,7 +1232,7 @@
         <v>13</v>
       </c>
       <c r="E20">
-        <v>0.22</v>
+        <v>0.8</v>
       </c>
       <c r="F20">
         <v>51756</v>
@@ -1251,10 +1255,10 @@
         <v>9</v>
       </c>
       <c r="E21">
-        <v>0.41</v>
+        <v>0.2</v>
       </c>
       <c r="F21">
-        <v>11111</v>
+        <v>434433</v>
       </c>
       <c r="G21" t="b">
         <v>0</v>
@@ -1274,10 +1278,10 @@
         <v>9</v>
       </c>
       <c r="E22">
-        <v>0.22</v>
+        <v>0.2</v>
       </c>
       <c r="F22">
-        <v>51756</v>
+        <v>434343</v>
       </c>
       <c r="G22" s="2" t="b">
         <v>0</v>
@@ -1297,10 +1301,10 @@
         <v>13</v>
       </c>
       <c r="E23">
-        <v>0.41</v>
+        <v>0.4</v>
       </c>
       <c r="F23">
-        <v>11111</v>
+        <v>434343</v>
       </c>
       <c r="G23" s="2" t="b">
         <v>0</v>
@@ -1320,10 +1324,10 @@
         <v>14</v>
       </c>
       <c r="E24">
-        <v>0.22</v>
+        <v>0.4</v>
       </c>
       <c r="F24">
-        <v>51756</v>
+        <v>434</v>
       </c>
       <c r="G24" s="2" t="b">
         <v>0</v>
@@ -1343,10 +1347,10 @@
         <v>13</v>
       </c>
       <c r="E25">
-        <v>0.41</v>
+        <v>0.56000000000000005</v>
       </c>
       <c r="F25">
-        <v>11111</v>
+        <v>7658</v>
       </c>
       <c r="G25" s="2" t="b">
         <v>0</v>
@@ -1366,10 +1370,10 @@
         <v>9</v>
       </c>
       <c r="E26">
-        <v>0.22</v>
+        <v>0.44</v>
       </c>
       <c r="F26">
-        <v>51756</v>
+        <v>874678</v>
       </c>
       <c r="G26" s="2" t="b">
         <v>0</v>
@@ -1389,13 +1393,13 @@
         <v>15</v>
       </c>
       <c r="E27">
-        <v>0.41</v>
+        <v>0.4</v>
       </c>
       <c r="F27">
-        <v>11111</v>
+        <v>232323</v>
       </c>
       <c r="G27" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="28" spans="1:7">
@@ -1412,10 +1416,10 @@
         <v>14</v>
       </c>
       <c r="E28">
-        <v>0.22</v>
+        <v>0.2</v>
       </c>
       <c r="F28">
-        <v>51756</v>
+        <v>4564</v>
       </c>
       <c r="G28" s="2" t="b">
         <v>0</v>
@@ -1435,10 +1439,10 @@
         <v>15</v>
       </c>
       <c r="E29">
-        <v>0.41</v>
+        <v>0.2</v>
       </c>
       <c r="F29">
-        <v>11111</v>
+        <v>5456</v>
       </c>
       <c r="G29" s="2" t="b">
         <v>0</v>
@@ -1458,10 +1462,10 @@
         <v>9</v>
       </c>
       <c r="E30">
-        <v>0.22</v>
+        <v>0.2</v>
       </c>
       <c r="F30">
-        <v>51756</v>
+        <v>5455</v>
       </c>
       <c r="G30" s="2" t="b">
         <v>0</v>
@@ -1481,10 +1485,10 @@
         <v>13</v>
       </c>
       <c r="E31">
-        <v>0.41</v>
+        <v>0.2</v>
       </c>
       <c r="F31">
-        <v>11111</v>
+        <v>45454</v>
       </c>
       <c r="G31" s="2" t="b">
         <v>0</v>
@@ -1504,10 +1508,10 @@
         <v>9</v>
       </c>
       <c r="E32">
-        <v>0.22</v>
+        <v>0.8</v>
       </c>
       <c r="F32">
-        <v>51756</v>
+        <v>45454</v>
       </c>
       <c r="G32" s="2" t="b">
         <v>0</v>
@@ -1527,10 +1531,10 @@
         <v>9</v>
       </c>
       <c r="E33">
-        <v>0.41</v>
+        <v>0.9</v>
       </c>
       <c r="F33">
-        <v>11111</v>
+        <v>6666</v>
       </c>
       <c r="G33" s="2" t="b">
         <v>0</v>
@@ -1550,10 +1554,10 @@
         <v>15</v>
       </c>
       <c r="E34">
-        <v>0.22</v>
+        <v>0.1</v>
       </c>
       <c r="F34">
-        <v>51756</v>
+        <v>443</v>
       </c>
       <c r="G34" s="2" t="b">
         <v>0</v>

</xml_diff>

<commit_message>
council update, added winners
</commit_message>
<xml_diff>
--- a/results/council-workbook.xlsx
+++ b/results/council-workbook.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26929"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27127"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="24040" yWindow="2660" windowWidth="27280" windowHeight="19480" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -268,6 +268,7 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -323,8 +324,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="85">
+  <cellStyleXfs count="87">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -417,7 +420,7 @@
     <xf numFmtId="3" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="85">
+  <cellStyles count="87">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -460,6 +463,7 @@
     <cellStyle name="Followed Hyperlink" xfId="80" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="82" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="84" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="86" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -502,6 +506,7 @@
     <cellStyle name="Hyperlink" xfId="79" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="81" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="83" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="85" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -834,7 +839,7 @@
   <dimension ref="A1:G40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F33" sqref="F33"/>
+      <selection sqref="A1:G34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0"/>
@@ -974,7 +979,7 @@
         <v>154158</v>
       </c>
       <c r="G6" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="17">
@@ -997,7 +1002,7 @@
         <v>11491</v>
       </c>
       <c r="G7" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="17">
@@ -1043,7 +1048,7 @@
         <v>12116</v>
       </c>
       <c r="G9" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="17">
@@ -1089,7 +1094,7 @@
         <v>13383</v>
       </c>
       <c r="G11" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="17">
@@ -1152,13 +1157,13 @@
         <v>9</v>
       </c>
       <c r="E14">
-        <v>0.89</v>
+        <v>0.88</v>
       </c>
       <c r="F14" s="3">
         <v>14646</v>
       </c>
       <c r="G14" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="17">
@@ -1175,13 +1180,13 @@
         <v>9</v>
       </c>
       <c r="E15">
-        <v>0.91</v>
+        <v>0.9</v>
       </c>
       <c r="F15" s="3">
         <v>12481</v>
       </c>
       <c r="G15" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="17">
@@ -1227,7 +1232,7 @@
         <v>11667</v>
       </c>
       <c r="G17" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="17">
@@ -1319,7 +1324,7 @@
         <v>14863</v>
       </c>
       <c r="G21" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="17">
@@ -1342,7 +1347,7 @@
         <v>10279</v>
       </c>
       <c r="G22" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="23" spans="1:7" ht="17">
@@ -1434,7 +1439,7 @@
         <v>7560</v>
       </c>
       <c r="G26" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="27" spans="1:7" ht="17">
@@ -1526,7 +1531,7 @@
         <v>8113</v>
       </c>
       <c r="G30" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="31" spans="1:7" ht="17">
@@ -1572,7 +1577,7 @@
         <v>11049</v>
       </c>
       <c r="G32" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="33" spans="1:7" ht="17">
@@ -1589,13 +1594,13 @@
         <v>9</v>
       </c>
       <c r="E33">
-        <v>0.92</v>
+        <v>0.91</v>
       </c>
       <c r="F33" s="3">
         <v>13823</v>
       </c>
       <c r="G33" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="34" spans="1:7" ht="17">

</xml_diff>